<commit_message>
fixed error in generation of two tables
</commit_message>
<xml_diff>
--- a/tables/table3a.xlsx
+++ b/tables/table3a.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="24030"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="20" windowWidth="16100" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -57,8 +52,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -409,19 +404,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:K1048576"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="1" width="16.6640625" customWidth="1"/>
-    <col min="6" max="6" width="12.5" customWidth="1"/>
-    <col min="11" max="11" width="15.83203125" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:11">
       <c r="B1" s="1" t="s">
@@ -463,31 +451,31 @@
         <v>10</v>
       </c>
       <c r="C2" s="2">
-        <v>0.93500000000000005</v>
+        <v>0.935</v>
       </c>
       <c r="D2" s="2">
-        <v>0.89100000000000001</v>
+        <v>0.908</v>
       </c>
       <c r="E2" s="2">
-        <v>0.93799999999999994</v>
+        <v>0.944</v>
       </c>
       <c r="F2" s="2">
-        <v>0.93600000000000005</v>
+        <v>0.942</v>
       </c>
       <c r="G2" s="2">
-        <v>0.93</v>
+        <v>0.939</v>
       </c>
       <c r="H2" s="2">
-        <v>0.92600000000000005</v>
+        <v>0.945</v>
       </c>
       <c r="I2" s="2">
-        <v>0.88900000000000001</v>
+        <v>0.909</v>
       </c>
       <c r="J2" s="2">
-        <v>0.93300000000000005</v>
+        <v>0.943</v>
       </c>
       <c r="K2" s="2">
-        <v>0.92500000000000004</v>
+        <v>0.941</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -501,28 +489,28 @@
         <v>10</v>
       </c>
       <c r="D3" s="2">
-        <v>0.89900000000000002</v>
+        <v>0.915</v>
       </c>
       <c r="E3" s="2">
-        <v>0.94799999999999995</v>
+        <v>0.94</v>
       </c>
       <c r="F3" s="2">
-        <v>0.95</v>
+        <v>0.945</v>
       </c>
       <c r="G3" s="2">
-        <v>0.93400000000000005</v>
+        <v>0.934</v>
       </c>
       <c r="H3" s="2">
-        <v>0.93100000000000005</v>
+        <v>0.942</v>
       </c>
       <c r="I3" s="2">
-        <v>0.89500000000000002</v>
+        <v>0.918</v>
       </c>
       <c r="J3" s="2">
-        <v>0.94099999999999995</v>
+        <v>0.944</v>
       </c>
       <c r="K3" s="2">
-        <v>0.92700000000000005</v>
+        <v>0.949</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -539,25 +527,25 @@
         <v>10</v>
       </c>
       <c r="E4" s="2">
-        <v>0.90800000000000003</v>
+        <v>0.917</v>
       </c>
       <c r="F4" s="2">
-        <v>0.89900000000000002</v>
+        <v>0.91</v>
       </c>
       <c r="G4" s="2">
-        <v>0.878</v>
+        <v>0.926</v>
       </c>
       <c r="H4" s="2">
-        <v>0.88500000000000001</v>
+        <v>0.913</v>
       </c>
       <c r="I4" s="2">
-        <v>0.95199999999999996</v>
+        <v>0.95</v>
       </c>
       <c r="J4" s="2">
-        <v>0.89700000000000002</v>
+        <v>0.917</v>
       </c>
       <c r="K4" s="2">
-        <v>0.878</v>
+        <v>0.92</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -577,22 +565,22 @@
         <v>10</v>
       </c>
       <c r="F5" s="2">
-        <v>0.95299999999999996</v>
+        <v>0.94</v>
       </c>
       <c r="G5" s="2">
-        <v>0.93799999999999994</v>
+        <v>0.938</v>
       </c>
       <c r="H5" s="2">
-        <v>0.93600000000000005</v>
+        <v>0.945</v>
       </c>
       <c r="I5" s="2">
-        <v>0.90500000000000003</v>
+        <v>0.914</v>
       </c>
       <c r="J5" s="2">
-        <v>0.94499999999999995</v>
+        <v>0.938</v>
       </c>
       <c r="K5" s="2">
-        <v>0.92800000000000005</v>
+        <v>0.942</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -615,19 +603,19 @@
         <v>10</v>
       </c>
       <c r="G6" s="2">
-        <v>0.93700000000000006</v>
+        <v>0.934</v>
       </c>
       <c r="H6" s="2">
-        <v>0.94</v>
+        <v>0.943</v>
       </c>
       <c r="I6" s="2">
-        <v>0.89400000000000002</v>
+        <v>0.907</v>
       </c>
       <c r="J6" s="2">
-        <v>0.94099999999999995</v>
+        <v>0.942</v>
       </c>
       <c r="K6" s="2">
-        <v>0.93200000000000005</v>
+        <v>0.941</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -653,16 +641,16 @@
         <v>10</v>
       </c>
       <c r="H7" s="2">
-        <v>0.94199999999999995</v>
+        <v>0.938</v>
       </c>
       <c r="I7" s="2">
-        <v>0.872</v>
+        <v>0.92</v>
       </c>
       <c r="J7" s="2">
-        <v>0.93899999999999995</v>
+        <v>0.939</v>
       </c>
       <c r="K7" s="2">
-        <v>0.93799999999999994</v>
+        <v>0.941</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -691,13 +679,13 @@
         <v>10</v>
       </c>
       <c r="I8" s="2">
-        <v>0.88800000000000001</v>
+        <v>0.909</v>
       </c>
       <c r="J8" s="2">
-        <v>0.93899999999999995</v>
+        <v>0.946</v>
       </c>
       <c r="K8" s="2">
-        <v>0.94799999999999995</v>
+        <v>0.947</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -729,10 +717,10 @@
         <v>10</v>
       </c>
       <c r="J9" s="2">
-        <v>0.89100000000000001</v>
+        <v>0.917</v>
       </c>
       <c r="K9" s="2">
-        <v>0.879</v>
+        <v>0.924</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -767,7 +755,7 @@
         <v>10</v>
       </c>
       <c r="K10" s="2">
-        <v>0.93300000000000005</v>
+        <v>0.945</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -807,10 +795,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>